<commit_message>
acrescenta nomes dos estados
</commit_message>
<xml_diff>
--- a/dados/dados-originais/tab_ufs.xlsx
+++ b/dados/dados-originais/tab_ufs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago.pereira\Documents\GitHub\estatais-estados\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tchiluanda/Documents/GitHub/estatais-estados-2020/dados/dados-originais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7753F2B6-F3B5-4864-9B38-1ADC43AF5BB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28A6AC0-98FA-484B-98F6-08DB8A0AC2AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{06E5B434-546D-441A-8AD3-4681C62FB42B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24240" windowHeight="13140" xr2:uid="{06E5B434-546D-441A-8AD3-4681C62FB42B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
-  <si>
-    <t>UF</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>RO</t>
   </si>
@@ -139,6 +136,93 @@
   </si>
   <si>
     <t>Centro-oeste</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Nome_estado</t>
+  </si>
+  <si>
+    <t>Rondônia</t>
+  </si>
+  <si>
+    <t>Acre</t>
+  </si>
+  <si>
+    <t>Amazonas</t>
+  </si>
+  <si>
+    <t>Roraima</t>
+  </si>
+  <si>
+    <t>Pará</t>
+  </si>
+  <si>
+    <t>Amapá</t>
+  </si>
+  <si>
+    <t>Tocantins</t>
+  </si>
+  <si>
+    <t>Maranhão</t>
+  </si>
+  <si>
+    <t>Piauí</t>
+  </si>
+  <si>
+    <t>Ceará</t>
+  </si>
+  <si>
+    <t>Rio Grande do Norte</t>
+  </si>
+  <si>
+    <t>Paraíba</t>
+  </si>
+  <si>
+    <t>Pernambuco</t>
+  </si>
+  <si>
+    <t>Alagoas</t>
+  </si>
+  <si>
+    <t>Sergipe</t>
+  </si>
+  <si>
+    <t>Bahia</t>
+  </si>
+  <si>
+    <t>Minas gerais</t>
+  </si>
+  <si>
+    <t>Espiríto Santo</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>Paraná</t>
+  </si>
+  <si>
+    <t>Santa Catarina</t>
+  </si>
+  <si>
+    <t>Rio Grande do Sul</t>
+  </si>
+  <si>
+    <t>Mato Grosso do Sul</t>
+  </si>
+  <si>
+    <t>Mato Grosso</t>
+  </si>
+  <si>
+    <t>Goiás</t>
+  </si>
+  <si>
+    <t>Distrito Federal</t>
   </si>
 </sst>
 </file>
@@ -490,406 +574,493 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831FC411-1B9D-4464-BA26-4414F7B8ECF3}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26">
+        <v>61</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28">
+        <v>63</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28">
         <v>5</v>
       </c>
     </row>

</xml_diff>